<commit_message>
fix: loading and saving files
</commit_message>
<xml_diff>
--- a/tests/6_save.xlsx
+++ b/tests/6_save.xlsx
@@ -95,9 +95,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode=""/>
-    <numFmt numFmtId="1" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="1">
+    <numFmt numFmtId="50" formatCode="#,##0.00%;(#,##0.00%)"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -281,135 +280,135 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="39" fontId="9" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="9" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="9" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="39" fontId="11" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="50" fontId="13" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="50" fontId="13" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="50" fontId="13" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="5" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="39" fontId="10" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="39" fontId="15" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="15" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="15" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="39" fontId="16" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="16" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="16" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="10" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="10" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="10" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="39" fontId="10" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -700,6 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultColWidth="3.53125" defaultRowHeight="17.4" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="27.50390625" style="1" customWidth="1"/>
@@ -734,6 +738,11 @@
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row>
       <c r="A8" s="8" t="s">
@@ -742,8 +751,13 @@
       <c r="B8" s="9">
         <v>2017</v>
       </c>
-    </row>
-    <row>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row>
+      <c r="A9" s="8"/>
       <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
@@ -864,6 +878,11 @@
       <c r="A14" s="27" t="s">
         <v>15</v>
       </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
     </row>
     <row>
       <c r="A15" s="29" t="s">
@@ -984,21 +1003,41 @@
       <c r="A20" s="26" t="s">
         <v>21</v>
       </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
     </row>
     <row>
       <c r="A21" s="26" t="s">
         <v>22</v>
       </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="39"/>
     </row>
     <row>
       <c r="A22" s="26" t="s">
         <v>23</v>
       </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="39"/>
     </row>
     <row>
       <c r="A23" s="26" t="s">
         <v>24</v>
       </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
     </row>
     <row>
       <c r="A24" s="26" t="s">
@@ -1029,14 +1068,27 @@
       <c r="A25" s="26" t="s">
         <v>26</v>
       </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
+    </row>
+    <row>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B8:F8"/>
     <mergeCell ref="A7:F7"/>
   </mergeCells>
 </worksheet>

</xml_diff>

<commit_message>
feat(funcs): add price and pricemat
</commit_message>
<xml_diff>
--- a/tests/6_save.xlsx
+++ b/tests/6_save.xlsx
@@ -1084,12 +1084,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A7:F7"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A7:F7"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: wrap cache with RefCell
</commit_message>
<xml_diff>
--- a/tests/6_save.xlsx
+++ b/tests/6_save.xlsx
@@ -1084,10 +1084,10 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A8:A9"/>
   </mergeCells>

</xml_diff>

<commit_message>
fix: save and load row infos
</commit_message>
<xml_diff>
--- a/tests/6_save.xlsx
+++ b/tests/6_save.xlsx
@@ -107,18 +107,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color auto="1"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color auto="1"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color auto="1"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color auto="1"/>
-      <sz val="10"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -280,9 +280,9 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -408,7 +408,7 @@
     <xf numFmtId="39" fontId="10" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -706,35 +706,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.53125" defaultRowHeight="17.4" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.50390625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.50390625" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row>
-      <c r="A1" s="3" t="s">
+    <row s="2" customFormat="1" ht="17.4" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="1" ht="20.625">
+    <row r="3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row>
+    <row ht="20.625" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row>
+    <row ht="20.625" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" s="1" ht="17.4">
+    <row r="7">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row>
+    <row ht="17.4" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="11" t="s">
         <v>6</v>
@@ -774,7 +774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
@@ -799,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
@@ -849,7 +849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>14</v>
       </c>
@@ -874,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>15</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A15" s="29" t="s">
         <v>16</v>
       </c>
@@ -909,7 +909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>17</v>
       </c>
@@ -934,7 +934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A17" s="26" t="s">
         <v>18</v>
       </c>
@@ -959,7 +959,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A18" s="26" t="s">
         <v>19</v>
       </c>
@@ -979,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A19" s="26" t="s">
         <v>20</v>
       </c>
@@ -999,7 +999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A20" s="26" t="s">
         <v>21</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="E20" s="38"/>
       <c r="F20" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>22</v>
       </c>
@@ -1019,7 +1019,7 @@
       <c r="E21" s="38"/>
       <c r="F21" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="E22" s="38"/>
       <c r="F22" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>24</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="E23" s="38"/>
       <c r="F23" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>25</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>26</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="E25" s="38"/>
       <c r="F25" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -1085,11 +1085,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: save and load row infos (#180)
</commit_message>
<xml_diff>
--- a/tests/6_save.xlsx
+++ b/tests/6_save.xlsx
@@ -107,18 +107,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color auto="1"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color auto="1"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color auto="1"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color auto="1"/>
-      <sz val="10"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -280,9 +280,9 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="1" borderId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -408,7 +408,7 @@
     <xf numFmtId="39" fontId="10" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -706,35 +706,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.53125" defaultRowHeight="17.4" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.50390625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.50390625" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row>
-      <c r="A1" s="3" t="s">
+    <row s="2" customFormat="1" ht="17.4" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="1" ht="20.625">
+    <row r="3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row>
+    <row ht="20.625" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row>
+    <row ht="20.625" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" s="1" ht="17.4">
+    <row r="7">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row>
+    <row ht="17.4" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="11" t="s">
         <v>6</v>
@@ -774,7 +774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
@@ -799,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
@@ -824,7 +824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
@@ -849,7 +849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>14</v>
       </c>
@@ -874,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>15</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A15" s="29" t="s">
         <v>16</v>
       </c>
@@ -909,7 +909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>17</v>
       </c>
@@ -934,7 +934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A17" s="26" t="s">
         <v>18</v>
       </c>
@@ -959,7 +959,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A18" s="26" t="s">
         <v>19</v>
       </c>
@@ -979,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A19" s="26" t="s">
         <v>20</v>
       </c>
@@ -999,7 +999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A20" s="26" t="s">
         <v>21</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="E20" s="38"/>
       <c r="F20" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>22</v>
       </c>
@@ -1019,7 +1019,7 @@
       <c r="E21" s="38"/>
       <c r="F21" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="E22" s="38"/>
       <c r="F22" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>24</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="E23" s="38"/>
       <c r="F23" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>25</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>26</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="E25" s="38"/>
       <c r="F25" s="39"/>
     </row>
-    <row>
+    <row ht="21.375" customHeight="1">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -1085,11 +1085,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: update gents and rename
</commit_message>
<xml_diff>
--- a/tests/6_save.xlsx
+++ b/tests/6_save.xlsx
@@ -1084,12 +1084,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="B8:F8"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>